<commit_message>
fixed R9 to 825ohms
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="180">
   <si>
     <t>http://www.dipmicro.com/store/index.php?act=viewProd&amp;productCode=CON-MICROSD1</t>
   </si>
@@ -547,13 +547,22 @@
   </si>
   <si>
     <t>Price for 100</t>
+  </si>
+  <si>
+    <t>825ohm</t>
+  </si>
+  <si>
+    <t>311-825HRCT-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/RC0603FR-07825RL/311-825HRCT-ND/730352</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -565,6 +574,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -591,9 +607,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -896,10 +913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1449,85 +1466,78 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22">
-        <f>A22 * B1 * B2</f>
-        <v>110.00000000000001</v>
-      </c>
-      <c r="C22" t="s">
-        <v>160</v>
+        <v>110</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>178</v>
       </c>
       <c r="D22">
-        <v>0.40500000000000003</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="F22" t="s">
-        <v>75</v>
+        <v>177</v>
       </c>
       <c r="G22" t="s">
-        <v>76</v>
-      </c>
-      <c r="H22" t="s">
-        <v>77</v>
-      </c>
-      <c r="I22" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B23">
         <f>A23 * B1 * B2</f>
-        <v>550</v>
+        <v>110.00000000000001</v>
       </c>
       <c r="C23" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D23">
-        <v>8.6E-3</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F23" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G23" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="H23" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="I23" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B24">
         <f>A24 * B1 * B2</f>
-        <v>220.00000000000003</v>
+        <v>550</v>
       </c>
       <c r="C24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D24">
-        <v>4.0000000000000001E-3</v>
+        <v>8.6E-3</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="F24">
-        <v>22</v>
+        <v>161</v>
+      </c>
+      <c r="F24" t="s">
+        <v>80</v>
       </c>
       <c r="G24" t="s">
         <v>81</v>
@@ -1541,23 +1551,23 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B25">
         <f>A25 * B1 * B2</f>
-        <v>330</v>
+        <v>220.00000000000003</v>
       </c>
       <c r="C25" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D25">
-        <v>4.7999999999999996E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F25">
-        <v>330</v>
+        <v>22</v>
       </c>
       <c r="G25" t="s">
         <v>81</v>
@@ -1571,23 +1581,23 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B26">
-        <f>A26*B1*B2</f>
+        <f>A26 * B1 * B2</f>
+        <v>220.00000000000003</v>
+      </c>
+      <c r="C26" t="s">
+        <v>166</v>
+      </c>
+      <c r="D26">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F26">
         <v>330</v>
-      </c>
-      <c r="C26" t="s">
-        <v>168</v>
-      </c>
-      <c r="D26">
-        <v>3.16E-3</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F26" t="s">
-        <v>93</v>
       </c>
       <c r="G26" t="s">
         <v>81</v>
@@ -1601,32 +1611,32 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B27">
-        <f>A27 * B1*B2</f>
-        <v>110.00000000000001</v>
+        <f>A27*B1*B2</f>
+        <v>330</v>
       </c>
       <c r="C27" t="s">
-        <v>117</v>
+        <v>168</v>
       </c>
       <c r="D27">
-        <v>0.41</v>
+        <v>3.16E-3</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>116</v>
+        <v>167</v>
       </c>
       <c r="F27" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="G27" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="H27" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="I27" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1634,23 +1644,29 @@
         <v>1</v>
       </c>
       <c r="B28">
-        <f>A28*B1*B2</f>
+        <f>A28 * B1*B2</f>
         <v>110.00000000000001</v>
       </c>
+      <c r="C28" t="s">
+        <v>117</v>
+      </c>
       <c r="D28">
-        <v>0.24</v>
+        <v>0.41</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="F28" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G28" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H28" t="s">
-        <v>107</v>
+        <v>104</v>
+      </c>
+      <c r="I28" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1661,26 +1677,20 @@
         <f>A29*B1*B2</f>
         <v>110.00000000000001</v>
       </c>
-      <c r="C29" t="s">
-        <v>119</v>
-      </c>
       <c r="D29">
-        <v>0.4</v>
+        <v>0.24</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>118</v>
+        <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G29" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H29" t="s">
-        <v>111</v>
-      </c>
-      <c r="I29" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1688,54 +1698,84 @@
         <v>1</v>
       </c>
       <c r="B30">
+        <f>A30*B1*B2</f>
+        <v>110.00000000000001</v>
+      </c>
+      <c r="C30" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30">
+        <v>0.4</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F30" t="s">
         <v>110</v>
       </c>
-      <c r="C30" t="s">
+      <c r="G30" t="s">
+        <v>111</v>
+      </c>
+      <c r="H30" t="s">
+        <v>111</v>
+      </c>
+      <c r="I30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>110</v>
+      </c>
+      <c r="C31" t="s">
         <v>172</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>174</v>
-      </c>
-      <c r="D32">
-        <f>SUM(D4:D31)</f>
-        <v>19.707640000000005</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D33">
-        <v>29</v>
+        <f>SUM(D4:D32)</f>
+        <v>19.713640000000005</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>175</v>
+      </c>
+      <c r="D34">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>173</v>
       </c>
-      <c r="D34">
+      <c r="D35">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>176</v>
       </c>
-      <c r="D36">
-        <f>(D32*B1*B2) +(D33*B1*B2) + D34</f>
-        <v>5402.840400000001</v>
+      <c r="D37">
+        <f>(D33*B1*B2) +(D34*B1*B2) + D35</f>
+        <v>5403.5004000000008</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E28" r:id="rId1"/>
-    <hyperlink ref="E27" r:id="rId2"/>
-    <hyperlink ref="E29" r:id="rId3"/>
+    <hyperlink ref="E29" r:id="rId1"/>
+    <hyperlink ref="E28" r:id="rId2"/>
+    <hyperlink ref="E30" r:id="rId3"/>
     <hyperlink ref="E5" r:id="rId4"/>
     <hyperlink ref="E6" r:id="rId5"/>
     <hyperlink ref="E7" r:id="rId6"/>
@@ -1751,11 +1791,12 @@
     <hyperlink ref="E17" r:id="rId16"/>
     <hyperlink ref="E18" r:id="rId17"/>
     <hyperlink ref="E21" r:id="rId18"/>
-    <hyperlink ref="E22" r:id="rId19"/>
-    <hyperlink ref="E23" r:id="rId20"/>
-    <hyperlink ref="E24" r:id="rId21"/>
-    <hyperlink ref="E25" r:id="rId22"/>
-    <hyperlink ref="E26" r:id="rId23"/>
+    <hyperlink ref="E23" r:id="rId19"/>
+    <hyperlink ref="E24" r:id="rId20"/>
+    <hyperlink ref="E25" r:id="rId21"/>
+    <hyperlink ref="E26" r:id="rId22"/>
+    <hyperlink ref="E27" r:id="rId23"/>
+    <hyperlink ref="E22" r:id="rId24" display="http://www.digikey.com/product-detail/en/ERJ-3EKF8250V/P825HDKR-ND/576362"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>